<commit_message>
bug fix (separator), white space class
</commit_message>
<xml_diff>
--- a/TestProject/TestProject/wwwroot/upload/template_test_graduate.xlsx
+++ b/TestProject/TestProject/wwwroot/upload/template_test_graduate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\GraduationAssesment\TestProject\TestProject\wwwroot\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/GraduationAssessment/GraduationAssesment/TestProject/TestProject/wwwroot/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFAFA9D-2221-4EF9-B27D-F01C29753860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECD6D4E-9B6F-B74C-803A-4F46F7BCECC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="30960" windowHeight="12108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="30960" windowHeight="12100" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="전체질문목록" sheetId="1" r:id="rId1"/>
@@ -637,10 +637,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CSE4074</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CSE4067</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -657,10 +653,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>공개SW프로젝트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>선과수행문화2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -686,6 +678,14 @@
   </si>
   <si>
     <t>불교와인간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSE2020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주니어디자인프로젝트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -693,7 +693,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1258,22 +1258,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" style="4"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="4"/>
     <col min="3" max="3" width="67" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="46.8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="48">
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="B9" s="4">
         <v>8</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7">
       <c r="B10" s="4">
         <v>9</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="B11" s="4">
         <v>10</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7">
       <c r="B12" s="4">
         <v>11</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7">
       <c r="B13" s="4">
         <v>12</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="B14" s="4">
         <v>13</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="B15" s="4">
         <v>14</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="B16" s="4">
         <v>15</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7">
       <c r="B18" s="4">
         <v>17</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7">
       <c r="B19" s="4">
         <v>18</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7">
       <c r="B20" s="4">
         <v>19</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7">
       <c r="B21" s="4">
         <v>20</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7">
       <c r="B22" s="4">
         <v>21</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7">
       <c r="B23" s="4">
         <v>22</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7">
       <c r="B24" s="4">
         <v>23</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7">
       <c r="B26" s="4">
         <v>25</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7">
       <c r="B27" s="4">
         <v>26</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7">
       <c r="B28" s="4">
         <v>27</v>
       </c>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7">
       <c r="B29" s="4">
         <v>28</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7">
       <c r="B30" s="4">
         <v>29</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7">
       <c r="B31" s="4">
         <v>30</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7">
       <c r="B32" s="4">
         <v>31</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="62.4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="48">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="62.4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="48">
       <c r="B34" s="4">
         <v>33</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7">
       <c r="B35" s="4">
         <v>34</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7">
       <c r="B36" s="4">
         <v>35</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7">
       <c r="B37" s="4">
         <v>36</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7">
       <c r="B38" s="4">
         <v>37</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7">
       <c r="B39" s="4">
         <v>38</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7">
       <c r="B40" s="4">
         <v>39</v>
       </c>
@@ -1992,18 +1992,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
@@ -2043,15 +2043,15 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="D3" s="5">
         <v>3</v>
@@ -2060,10 +2060,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="5">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -2073,7 +2073,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -2083,7 +2083,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -2093,7 +2093,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -2103,7 +2103,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -2123,7 +2123,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -2133,7 +2133,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -2143,7 +2143,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -2153,7 +2153,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:6" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2168,14 +2168,14 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
@@ -2215,15 +2215,15 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D3" s="27">
         <v>3</v>
@@ -2235,15 +2235,15 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>151</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>152</v>
       </c>
       <c r="D4" s="27">
         <v>3</v>
@@ -2255,7 +2255,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -2265,7 +2265,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -2275,7 +2275,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -2285,7 +2285,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -2295,7 +2295,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -2305,7 +2305,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -2315,7 +2315,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -2325,7 +2325,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -2335,7 +2335,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:6" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2350,7 +2350,7 @@
       <selection activeCell="I32" activeCellId="1" sqref="J23 I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
@@ -2360,7 +2360,7 @@
     <col min="13" max="13" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="28" t="s">
         <v>62</v>
       </c>
@@ -2382,7 +2382,7 @@
       <c r="K1" s="29"/>
       <c r="L1" s="29"/>
     </row>
-    <row r="2" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="28"/>
       <c r="B2" s="11" t="s">
         <v>59</v>
@@ -2418,7 +2418,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="4" t="s">
         <v>65</v>
       </c>
@@ -2448,7 +2448,7 @@
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
     </row>
-    <row r="4" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -2464,7 +2464,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -2480,7 +2480,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -2496,7 +2496,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -2512,7 +2512,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -2528,7 +2528,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -2544,7 +2544,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -2560,7 +2560,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -2576,7 +2576,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -2592,7 +2592,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A13" s="14">
         <v>10</v>
       </c>
@@ -2608,7 +2608,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:12" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
@@ -2630,7 +2630,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
@@ -2640,7 +2640,7 @@
     <col min="13" max="13" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="28" t="s">
         <v>62</v>
       </c>
@@ -2662,7 +2662,7 @@
       <c r="K1" s="29"/>
       <c r="L1" s="29"/>
     </row>
-    <row r="2" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="28"/>
       <c r="B2" s="11" t="s">
         <v>59</v>
@@ -2698,7 +2698,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="4" t="s">
         <v>65</v>
       </c>
@@ -2728,7 +2728,7 @@
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
     </row>
-    <row r="4" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -2744,7 +2744,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -2776,7 +2776,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -2792,7 +2792,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -2808,7 +2808,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -2824,7 +2824,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -2840,7 +2840,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -2856,7 +2856,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -2872,7 +2872,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="A13" s="13">
         <v>10</v>
       </c>
@@ -2888,7 +2888,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:12" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
@@ -2909,15 +2909,15 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -2967,7 +2967,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -2977,7 +2977,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -2987,7 +2987,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -2997,7 +2997,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -3007,7 +3007,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -3027,7 +3027,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -3037,7 +3037,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -3047,7 +3047,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -3057,7 +3057,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:6" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3072,12 +3072,12 @@
       <selection activeCell="B10" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
@@ -3111,15 +3111,15 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -3128,15 +3128,15 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
@@ -3145,7 +3145,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>99</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
@@ -3162,7 +3162,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>142</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D6" s="5">
         <v>2</v>
@@ -3179,7 +3179,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>143</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D7" s="5">
         <v>3</v>
@@ -3196,7 +3196,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -3239,7 +3239,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -3248,7 +3248,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -3257,7 +3257,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:5" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3273,12 +3273,12 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -3406,7 +3406,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -3415,7 +3415,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -3424,7 +3424,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -3433,7 +3433,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -3442,7 +3442,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:5" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3457,13 +3457,13 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -3540,7 +3540,7 @@
       <c r="D5" s="23"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -3558,7 +3558,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -3567,7 +3567,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -3576,7 +3576,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -3585,7 +3585,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -3594,7 +3594,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -3603,7 +3603,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:5" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3618,12 +3618,12 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -3768,7 +3768,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -3777,7 +3777,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -3786,7 +3786,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -3795,7 +3795,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:5" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3810,12 +3810,12 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -3858,7 +3858,7 @@
       <c r="D3" s="22"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -3867,7 +3867,7 @@
       <c r="D4" s="22"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -3876,7 +3876,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -3885,7 +3885,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -3894,7 +3894,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -3903,7 +3903,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -3912,7 +3912,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -3921,7 +3921,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -3930,7 +3930,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -3939,7 +3939,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:5" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3955,12 +3955,12 @@
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -4003,7 +4003,7 @@
       <c r="D3" s="22"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -4012,7 +4012,7 @@
       <c r="D4" s="22"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -4021,7 +4021,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -4030,7 +4030,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -4039,7 +4039,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -4048,7 +4048,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -4057,7 +4057,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -4066,7 +4066,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -4075,7 +4075,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -4084,7 +4084,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:5" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4100,14 +4100,14 @@
       <selection activeCell="B7" sqref="B7:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -4237,7 +4237,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -4247,7 +4247,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -4257,7 +4257,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -4267,7 +4267,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -4277,7 +4277,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -4287,7 +4287,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:6" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4303,14 +4303,14 @@
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
@@ -4350,7 +4350,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -4380,7 +4380,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -4390,7 +4390,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -4400,7 +4400,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -4410,7 +4410,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -4420,7 +4420,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -4430,7 +4430,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -4440,7 +4440,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -4450,7 +4450,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -4460,7 +4460,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:6" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>